<commit_message>
add week 1 slides
</commit_message>
<xml_diff>
--- a/syllabus/class_schedule.xlsx
+++ b/syllabus/class_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/judebayham/Documents/git_projects/arec-330/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D657CE5-8A73-8A4B-BEEB-25E25E71C5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAFB8E8-7AF1-0C45-B99E-4481B6F04211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36940" yWindow="1580" windowWidth="34560" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37020" yWindow="2580" windowWidth="34560" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sp2026" sheetId="6" r:id="rId1"/>
@@ -579,7 +579,7 @@
   <dimension ref="A1:E964"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -588,7 +588,7 @@
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
fixing broken link and updating schedule
</commit_message>
<xml_diff>
--- a/syllabus/class_schedule.xlsx
+++ b/syllabus/class_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/judebayham/Documents/git_projects/arec-330/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAFB8E8-7AF1-0C45-B99E-4481B6F04211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855F67DF-27AE-B948-87A6-1CA1E3045DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37020" yWindow="2580" windowWidth="34560" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16580" yWindow="1160" windowWidth="17920" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sp2026" sheetId="6" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>week</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Explanatory Data Analysis Part 2</t>
+  </si>
+  <si>
+    <t>Asking the right question</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
   <dimension ref="A1:E964"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -631,8 +634,8 @@
         <f>B2+7</f>
         <v>46050</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="C3" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
add rubrics; update schedules
</commit_message>
<xml_diff>
--- a/syllabus/class_schedule.xlsx
+++ b/syllabus/class_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/judebayham/Documents/git_projects/arec-330/syllabus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855F67DF-27AE-B948-87A6-1CA1E3045DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A98D42-4F01-5548-9742-1B601637C869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16580" yWindow="1160" windowWidth="17920" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12020" yWindow="680" windowWidth="17920" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sp2026" sheetId="6" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>week</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Asking the right question</t>
+  </si>
+  <si>
+    <t>Exploratory Data Analysis (Power BI)</t>
+  </si>
+  <si>
+    <t>Forecasting (asynchronous)</t>
   </si>
 </sst>
 </file>
@@ -231,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -252,6 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,7 +589,7 @@
   <dimension ref="A1:E964"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -684,8 +691,8 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -697,8 +704,8 @@
         <f t="shared" si="0"/>
         <v>46078</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
+      <c r="C7" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>9</v>

</xml_diff>